<commit_message>
group by custom interval?
</commit_message>
<xml_diff>
--- a/Insiderate/test.xlsx
+++ b/Insiderate/test.xlsx
@@ -192,7 +192,7 @@
   <dimension ref="A1:L367"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A5" activeCellId="0" pane="topLeft" sqref="A5"/>
+      <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -290,7 +290,7 @@
         <v>33.35</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
       <c r="A4" s="2" t="n">
         <v>41276</v>
       </c>
@@ -14141,12 +14141,13 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="G2" activeCellId="0" pane="topLeft" sqref="G2"/>
+      <selection activeCell="D6" activeCellId="0" pane="topLeft" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="9.09716599190283"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.2834008097166"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="14.1336032388664"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.7206477732794"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.5748987854251"/>
   </cols>

</xml_diff>